<commit_message>
Add female headers smt to bom
</commit_message>
<xml_diff>
--- a/openbci_wifi_bom.xlsx
+++ b/openbci_wifi_bom.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24960" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21900" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="openbci_wifi_bom" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="114">
   <si>
     <t>Quantity</t>
   </si>
@@ -285,6 +285,90 @@
   </si>
   <si>
     <t>MBR120VLSFT3G</t>
+  </si>
+  <si>
+    <t>New Parts</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/amphenol-fci/89898-308LF/609-3043-ND/1535456</t>
+  </si>
+  <si>
+    <t>Amphenol FCI</t>
+  </si>
+  <si>
+    <t>89898-308LF</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/products/en/connectors-interconnects/rectangular-connectors-headers-male-pins/314?k=&amp;pkeyword=&amp;pv88=2&amp;FV=fff802f3%2C1140003%2C1bf80001%2C1f940001%2C1f940005%2Cffe0013a&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>OpenBCI_Wifi_Shield:M20-8770242</t>
+  </si>
+  <si>
+    <t>Harwin</t>
+  </si>
+  <si>
+    <t>OpenBCI_Wifi_Shield:89898-308LF</t>
+  </si>
+  <si>
+    <t>M20-8770242</t>
+  </si>
+  <si>
+    <t>OpenBCI_Wifi_Shield:M20-8770442</t>
+  </si>
+  <si>
+    <t>M20-8770442</t>
+  </si>
+  <si>
+    <t>CONN_02X08_FEMALE</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P7, P8, P11</t>
+  </si>
+  <si>
+    <t>P1, P13, P14</t>
+  </si>
+  <si>
+    <t>http://portal.fciconnect.com/Comergent//fci/drawing/95278.pdf</t>
+  </si>
+  <si>
+    <t>95278-101A16LF</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/NPPC021KFXC-RC/S5633-ND/776092</t>
+  </si>
+  <si>
+    <t>Sullins Connector Solutions</t>
+  </si>
+  <si>
+    <t>OpenBCI_Wifi_Shield:95278-101A16LF</t>
+  </si>
+  <si>
+    <t>OpenBCI_Wifi_Shield:</t>
+  </si>
+  <si>
+    <t>CONN_02X08_MALE</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>NPTC021KFXC-RC</t>
+  </si>
+  <si>
+    <t>P4, P5, P6</t>
+  </si>
+  <si>
+    <t>P9, P10</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/NPTC041KFXC-RC/S5596-ND/776054</t>
+  </si>
+  <si>
+    <t>NPTC041KFXC-RC</t>
   </si>
 </sst>
 </file>
@@ -633,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1047,7 +1131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1067,7 +1151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1085,11 +1169,152 @@
       </c>
       <c r="H18">
         <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" t="s">
+        <v>93</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" t="s">
+        <v>91</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="J24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" t="s">
+        <v>95</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" t="s">
+        <v>105</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="J26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" t="s">
+        <v>106</v>
+      </c>
+      <c r="H27">
+        <v>3</v>
+      </c>
+      <c r="J27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="J28" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F10" r:id="rId1"/>
+    <hyperlink ref="F23" r:id="rId2"/>
+    <hyperlink ref="E26" r:id="rId3"/>
+    <hyperlink ref="F27" r:id="rId4"/>
+    <hyperlink ref="F28" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finish adding new parts to BOM
</commit_message>
<xml_diff>
--- a/openbci_wifi_bom.xlsx
+++ b/openbci_wifi_bom.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="107">
   <si>
     <t>Quantity</t>
   </si>
@@ -41,21 +41,9 @@
     <t>SPDT</t>
   </si>
   <si>
-    <t>P8,P7</t>
-  </si>
-  <si>
-    <t>CONN_01X08</t>
-  </si>
-  <si>
     <t>CONN_01X04</t>
   </si>
   <si>
-    <t>P4,P6,P5</t>
-  </si>
-  <si>
-    <t>Socket_Strip_Straight_1x02</t>
-  </si>
-  <si>
     <t>CONN_01X02</t>
   </si>
   <si>
@@ -80,15 +68,9 @@
     <t>10uF</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>MBR120</t>
   </si>
   <si>
-    <t>D2</t>
-  </si>
-  <si>
     <t>LED</t>
   </si>
   <si>
@@ -98,15 +80,9 @@
     <t>JST_RA_SMT</t>
   </si>
   <si>
-    <t>R1,R2,R4</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
     <t>1k</t>
   </si>
   <si>
@@ -170,30 +146,6 @@
     <t>OpenBCI:SSSS810701</t>
   </si>
   <si>
-    <t>Socket_Strip_Straight_1x08 0.1” pitch</t>
-  </si>
-  <si>
-    <t>Sullins</t>
-  </si>
-  <si>
-    <t>Socket_Strips:Socket_Strip_Straight_1x08</t>
-  </si>
-  <si>
-    <t>Socket_Strip_Straight_1x04 0.1” pitch</t>
-  </si>
-  <si>
-    <t>PPTC041LFBN-RC</t>
-  </si>
-  <si>
-    <t>Socket_Strips:Socket_Strip_Straight_1x04</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>P9,P10</t>
-  </si>
-  <si>
     <t>C4</t>
   </si>
   <si>
@@ -221,12 +173,6 @@
     <t>kicad-libraries-master:SOD-123FL</t>
   </si>
   <si>
-    <t>Socket_Strips:Socket_Strip_Straight_1x02</t>
-  </si>
-  <si>
-    <t>OpenBCI:JST_RA_SMT</t>
-  </si>
-  <si>
     <t>TO_SOT_Packages_SMD:SOT-23-5</t>
   </si>
   <si>
@@ -287,9 +233,6 @@
     <t>MBR120VLSFT3G</t>
   </si>
   <si>
-    <t>New Parts</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/amphenol-fci/89898-308LF/609-3043-ND/1535456</t>
   </si>
   <si>
@@ -347,28 +290,64 @@
     <t>OpenBCI_Wifi_Shield:95278-101A16LF</t>
   </si>
   <si>
-    <t>OpenBCI_Wifi_Shield:</t>
-  </si>
-  <si>
     <t>CONN_02X08_MALE</t>
   </si>
   <si>
     <t>P12</t>
   </si>
   <si>
-    <t>NPTC021KFXC-RC</t>
-  </si>
-  <si>
     <t>P4, P5, P6</t>
   </si>
   <si>
     <t>P9, P10</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/NPTC041KFXC-RC/S5596-ND/776054</t>
-  </si>
-  <si>
-    <t>NPTC041KFXC-RC</t>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/NPPC041KFXC-RC/S5635-ND/776094</t>
+  </si>
+  <si>
+    <t>NPPC041KFXC-RC</t>
+  </si>
+  <si>
+    <t>NPPC021KFXC-RC</t>
+  </si>
+  <si>
+    <t>OpenBCI_Wifi_Shield:NPPC021KFXC-RC</t>
+  </si>
+  <si>
+    <t>OpenBCI_Wifi_Shield:NPPC041KFXC-RC</t>
+  </si>
+  <si>
+    <t>SW4</t>
+  </si>
+  <si>
+    <t>CJS1200</t>
+  </si>
+  <si>
+    <t>DIP Switch</t>
+  </si>
+  <si>
+    <t>CJS-1200TA</t>
+  </si>
+  <si>
+    <t>Copal</t>
+  </si>
+  <si>
+    <t>OpenBCI:CJS-1200TA</t>
+  </si>
+  <si>
+    <t>D1,D4</t>
+  </si>
+  <si>
+    <t>D2,D3,D5</t>
+  </si>
+  <si>
+    <t>OpenBCI_Wifi_Shield:JST_RA_SMT</t>
+  </si>
+  <si>
+    <t>R1,R2,R5,R6,R7</t>
+  </si>
+  <si>
+    <t>R3,R4,R8</t>
   </si>
 </sst>
 </file>
@@ -717,14 +696,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="23.5" customWidth="1"/>
@@ -734,81 +714,85 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="G2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="3">
-        <v>2</v>
+        <v>44</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>50</v>
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="3">
+        <v>45</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
     </row>
@@ -817,21 +801,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="G4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" s="3">
-        <v>2</v>
+        <v>42</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -839,19 +827,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -859,25 +847,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>75</v>
+        <v>46</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="H6">
         <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -885,22 +876,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>75</v>
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -914,19 +905,19 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>75</v>
+      <c r="E8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -937,152 +928,152 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>59</v>
+        <v>78</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" t="s">
+        <v>74</v>
       </c>
       <c r="H9">
         <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>63</v>
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" t="s">
+        <v>72</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J10" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>58</v>
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" t="s">
+        <v>76</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>65</v>
+        <v>87</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" t="s">
+        <v>86</v>
       </c>
       <c r="H12">
         <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>69</v>
+        <v>89</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" t="s">
+        <v>94</v>
       </c>
       <c r="H13">
         <v>3</v>
       </c>
+      <c r="J13" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>69</v>
+        <v>90</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" t="s">
+        <v>95</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J14" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1090,231 +1081,187 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
+        <v>17</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16">
         <v>3</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="3" t="s">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17">
         <v>2</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" t="s">
-        <v>97</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G23" t="s">
-        <v>93</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="J23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" t="s">
-        <v>92</v>
-      </c>
-      <c r="G24" t="s">
-        <v>91</v>
-      </c>
-      <c r="H24">
-        <v>3</v>
-      </c>
-      <c r="J24" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>100</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>96</v>
-      </c>
-      <c r="F25" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" t="s">
-        <v>95</v>
-      </c>
-      <c r="H25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" t="s">
-        <v>107</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F26" t="s">
-        <v>88</v>
-      </c>
-      <c r="G26" t="s">
-        <v>105</v>
-      </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-      <c r="J26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G27" t="s">
-        <v>106</v>
-      </c>
-      <c r="H27">
-        <v>3</v>
-      </c>
-      <c r="J27" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="H28">
-        <v>2</v>
-      </c>
-      <c r="J28" t="s">
-        <v>112</v>
-      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E26" s="5"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E30" s="5"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E31" s="5"/>
+      <c r="F31" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F10" r:id="rId1"/>
-    <hyperlink ref="F23" r:id="rId2"/>
-    <hyperlink ref="E26" r:id="rId3"/>
-    <hyperlink ref="F27" r:id="rId4"/>
-    <hyperlink ref="F28" r:id="rId5"/>
+    <hyperlink ref="F6" r:id="rId1"/>
+    <hyperlink ref="F9" r:id="rId2"/>
+    <hyperlink ref="E12" r:id="rId3"/>
+    <hyperlink ref="F13" r:id="rId4"/>
+    <hyperlink ref="F14" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update bom with new parts
</commit_message>
<xml_diff>
--- a/openbci_wifi_bom.xlsx
+++ b/openbci_wifi_bom.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="110">
   <si>
     <t>Quantity</t>
   </si>
@@ -233,27 +233,12 @@
     <t>MBR120VLSFT3G</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/amphenol-fci/89898-308LF/609-3043-ND/1535456</t>
-  </si>
-  <si>
-    <t>Amphenol FCI</t>
-  </si>
-  <si>
-    <t>89898-308LF</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/products/en/connectors-interconnects/rectangular-connectors-headers-male-pins/314?k=&amp;pkeyword=&amp;pv88=2&amp;FV=fff802f3%2C1140003%2C1bf80001%2C1f940001%2C1f940005%2Cffe0013a&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
-  </si>
-  <si>
     <t>OpenBCI_Wifi_Shield:M20-8770242</t>
   </si>
   <si>
     <t>Harwin</t>
   </si>
   <si>
-    <t>OpenBCI_Wifi_Shield:89898-308LF</t>
-  </si>
-  <si>
     <t>M20-8770242</t>
   </si>
   <si>
@@ -275,21 +260,12 @@
     <t>P1, P13, P14</t>
   </si>
   <si>
-    <t>http://portal.fciconnect.com/Comergent//fci/drawing/95278.pdf</t>
-  </si>
-  <si>
-    <t>95278-101A16LF</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/NPPC021KFXC-RC/S5633-ND/776092</t>
   </si>
   <si>
     <t>Sullins Connector Solutions</t>
   </si>
   <si>
-    <t>OpenBCI_Wifi_Shield:95278-101A16LF</t>
-  </si>
-  <si>
     <t>CONN_02X08_MALE</t>
   </si>
   <si>
@@ -348,13 +324,46 @@
   </si>
   <si>
     <t>R3,R4,R8</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/harwin-inc/M20-8770242/M20-8770242-ND/3920067</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/harwin-inc/M20-8770442/952-2353-ND/3906342</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/NPPC082KFMS-RC/S5717-ND/776176</t>
+  </si>
+  <si>
+    <t>NPPC082KFMS-RC</t>
+  </si>
+  <si>
+    <t>OpenBCI_Wifi_Shield:NPPC082KFMS-RC</t>
+  </si>
+  <si>
+    <t>Datasheet</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/harwin-inc/M20-8750842/952-3162-ND/6559247</t>
+  </si>
+  <si>
+    <t>https://cdn.harwin.com/pdfs/M20-875.pdf</t>
+  </si>
+  <si>
+    <t>M20-8750842</t>
+  </si>
+  <si>
+    <t>OpenBCI_Wifi_Shield:M20-8750842</t>
+  </si>
+  <si>
+    <t>http://sullinscorp.com/drawings/103_NPxCxx2KFMx-RC,_10488-G.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -371,12 +380,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -388,6 +391,18 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -409,15 +424,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -696,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,7 +729,7 @@
     <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -743,525 +760,582 @@
       <c r="J1" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="K1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C7" t="s">
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="2">
+        <v>3</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="2">
+        <v>3</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="2">
+        <v>3</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="2">
+        <v>2</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="2">
+        <v>5</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="2">
+        <v>3</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" t="s">
-        <v>74</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="J9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" t="s">
-        <v>73</v>
-      </c>
-      <c r="G10" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10">
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="2">
+        <v>2</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" t="s">
-        <v>77</v>
-      </c>
-      <c r="F11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" t="s">
-        <v>76</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D18" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D12" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" t="s">
-        <v>86</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C19" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="D19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G13" t="s">
-        <v>94</v>
-      </c>
-      <c r="H13">
-        <v>3</v>
-      </c>
-      <c r="J13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H14">
-        <v>2</v>
-      </c>
-      <c r="J14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" t="s">
-        <v>98</v>
-      </c>
-      <c r="E19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" t="s">
-        <v>100</v>
-      </c>
-      <c r="G19" t="s">
-        <v>101</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E26" s="5"/>
-      <c r="F26" s="4"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E30" s="5"/>
-      <c r="F30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E31" s="5"/>
-      <c r="F31" s="4"/>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E26" s="4"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E30" s="4"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E31" s="4"/>
+      <c r="F31" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1"/>
-    <hyperlink ref="F9" r:id="rId2"/>
-    <hyperlink ref="E12" r:id="rId3"/>
-    <hyperlink ref="F13" r:id="rId4"/>
-    <hyperlink ref="F14" r:id="rId5"/>
+    <hyperlink ref="F13" r:id="rId2"/>
+    <hyperlink ref="F14" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bump version to 1.0.0 for first release
</commit_message>
<xml_diff>
--- a/openbci_wifi_bom.xlsx
+++ b/openbci_wifi_bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
   <si>
     <t>Quantity</t>
   </si>
@@ -35,9 +35,6 @@
     <t>SW3</t>
   </si>
   <si>
-    <t>SSSS810701</t>
-  </si>
-  <si>
     <t>SPDT</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>Alps</t>
   </si>
   <si>
-    <t>OpenBCI:SSSS810701</t>
-  </si>
-  <si>
     <t>Socket_Strip_Straight_1x08 0.1” pitch</t>
   </si>
   <si>
@@ -297,6 +291,15 @@
   </si>
   <si>
     <t>Dip switch</t>
+  </si>
+  <si>
+    <t>PCM12SMTR</t>
+  </si>
+  <si>
+    <t>C&amp;K Components</t>
+  </si>
+  <si>
+    <t>OpenBCI_Wifi_Shield:PCM12SMTR</t>
   </si>
 </sst>
 </file>
@@ -657,7 +660,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,34 +676,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -708,18 +711,18 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H2" s="3">
         <v>2</v>
@@ -730,22 +733,22 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="H3" s="3">
         <v>1</v>
@@ -756,18 +759,18 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H4" s="3">
         <v>2</v>
@@ -778,16 +781,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H5">
         <v>3</v>
@@ -798,22 +801,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -824,22 +827,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -850,22 +853,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -876,16 +879,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
         <v>52</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -896,28 +899,28 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -925,22 +928,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H11">
         <v>3</v>
@@ -951,22 +954,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -977,22 +980,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="G13" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H13">
         <v>5</v>
@@ -1003,22 +1006,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="G14" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -1029,16 +1032,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
         <v>27</v>
       </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" t="s">
-        <v>28</v>
-      </c>
       <c r="G15" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H15">
         <v>2</v>
@@ -1052,19 +1055,19 @@
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>2</v>
+        <v>88</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -1075,22 +1078,22 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -1101,16 +1104,16 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
         <v>24</v>
       </c>
-      <c r="C18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" t="s">
-        <v>25</v>
-      </c>
       <c r="G18" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -1121,16 +1124,16 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" t="s">
-        <v>31</v>
-      </c>
       <c r="G19" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H19">
         <v>1</v>

</xml_diff>